<commit_message>
Update words and add some things
</commit_message>
<xml_diff>
--- a/Allemand.xlsx
+++ b/Allemand.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hwalog\Documents\word_trainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A032FD5A-6FB7-4360-A197-11F0392A1D45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D462EC-CB15-4FCD-A5EA-9A5597FE44B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="606">
   <si>
     <t>Mot français</t>
   </si>
@@ -1771,6 +1771,78 @@
   </si>
   <si>
     <t>la connexion</t>
+  </si>
+  <si>
+    <t>überhaupt</t>
+  </si>
+  <si>
+    <t>en général</t>
+  </si>
+  <si>
+    <t>überhaupt nicht</t>
+  </si>
+  <si>
+    <t>pas du tout</t>
+  </si>
+  <si>
+    <t>verhindern</t>
+  </si>
+  <si>
+    <t>empêcher</t>
+  </si>
+  <si>
+    <t>derzeit</t>
+  </si>
+  <si>
+    <t>actuellement</t>
+  </si>
+  <si>
+    <t>ausschliesslich</t>
+  </si>
+  <si>
+    <t>exclusif</t>
+  </si>
+  <si>
+    <t>das Gefängnis</t>
+  </si>
+  <si>
+    <t>la prison</t>
+  </si>
+  <si>
+    <t>der Knast</t>
+  </si>
+  <si>
+    <t>la taule</t>
+  </si>
+  <si>
+    <t>schaffen</t>
+  </si>
+  <si>
+    <t>réussir</t>
+  </si>
+  <si>
+    <t>in alle Richtungen spritzen</t>
+  </si>
+  <si>
+    <t>gicler dans tous les sens</t>
+  </si>
+  <si>
+    <t>das Waschbecken</t>
+  </si>
+  <si>
+    <t>le lavabo</t>
+  </si>
+  <si>
+    <t>ausprobieren</t>
+  </si>
+  <si>
+    <t>essayer (mettre à l'épreuve)</t>
+  </si>
+  <si>
+    <t>verkalkt</t>
+  </si>
+  <si>
+    <t>entartré</t>
   </si>
 </sst>
 </file>
@@ -2105,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B293"/>
+  <dimension ref="A1:B305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="A294" sqref="A294"/>
+    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="A306" sqref="A306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4461,6 +4533,102 @@
         <v>581</v>
       </c>
     </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A295" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A296" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A297" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A298" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A299" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A300" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A301" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A302" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A303" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A304" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A305" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajoute de quoi s'entrainer sur les categories
</commit_message>
<xml_diff>
--- a/Allemand.xlsx
+++ b/Allemand.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hwalog\Documents\word_trainer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hwalog\files\word_trainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D462EC-CB15-4FCD-A5EA-9A5597FE44B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBEA0B1-BDAA-4BE4-B79B-ED4495379543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Categorie" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="951">
   <si>
     <t>Mot français</t>
   </si>
@@ -1843,6 +1843,1041 @@
   </si>
   <si>
     <t>entartré</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>situation</t>
+  </si>
+  <si>
+    <t>préférer</t>
+  </si>
+  <si>
+    <t>me reposer</t>
+  </si>
+  <si>
+    <t>regarder un film</t>
+  </si>
+  <si>
+    <t>s'entraîner</t>
+  </si>
+  <si>
+    <t>der Plan</t>
+  </si>
+  <si>
+    <t>die Situation</t>
+  </si>
+  <si>
+    <t>lieber mögen</t>
+  </si>
+  <si>
+    <t>ausruhen</t>
+  </si>
+  <si>
+    <t>ich habe das Gefühl</t>
+  </si>
+  <si>
+    <t>j'ai l'impression</t>
+  </si>
+  <si>
+    <t>die Zeit vertrödeln</t>
+  </si>
+  <si>
+    <t>perdre du temps</t>
+  </si>
+  <si>
+    <t>einen Film schauen</t>
+  </si>
+  <si>
+    <t>trainieren</t>
+  </si>
+  <si>
+    <t>lifestyle</t>
+  </si>
+  <si>
+    <t>raconter</t>
+  </si>
+  <si>
+    <t>s'amuser</t>
+  </si>
+  <si>
+    <t>Spass haben</t>
+  </si>
+  <si>
+    <t>die Lebensstil</t>
+  </si>
+  <si>
+    <t>die Gewohnheit</t>
+  </si>
+  <si>
+    <t>l'habitude</t>
+  </si>
+  <si>
+    <t>der Mitbewohner</t>
+  </si>
+  <si>
+    <t>le colocataire</t>
+  </si>
+  <si>
+    <t>erzählen</t>
+  </si>
+  <si>
+    <t>him</t>
+  </si>
+  <si>
+    <t>ca fait mal</t>
+  </si>
+  <si>
+    <t>gratter</t>
+  </si>
+  <si>
+    <t>tard</t>
+  </si>
+  <si>
+    <t>should</t>
+  </si>
+  <si>
+    <t>journal intime</t>
+  </si>
+  <si>
+    <t>je n'aurais pas du faire quelque chose</t>
+  </si>
+  <si>
+    <t>ich hätte nicht etwas machen sollen</t>
+  </si>
+  <si>
+    <t>ihn / ihm</t>
+  </si>
+  <si>
+    <t>Es tut weh</t>
+  </si>
+  <si>
+    <t>kratzen</t>
+  </si>
+  <si>
+    <t>spät</t>
+  </si>
+  <si>
+    <t>selbstbewusst</t>
+  </si>
+  <si>
+    <t>confiant, avec de l'assurance</t>
+  </si>
+  <si>
+    <t>sollen</t>
+  </si>
+  <si>
+    <t>das Tagebuch</t>
+  </si>
+  <si>
+    <t>Glückwunsch</t>
+  </si>
+  <si>
+    <t>félicitations</t>
+  </si>
+  <si>
+    <t>durant</t>
+  </si>
+  <si>
+    <t>ca m'a marqué</t>
+  </si>
+  <si>
+    <t>tâche</t>
+  </si>
+  <si>
+    <t>contrôler</t>
+  </si>
+  <si>
+    <t>während</t>
+  </si>
+  <si>
+    <t>Es hat micht geprägt</t>
+  </si>
+  <si>
+    <t>die Aufgabe</t>
+  </si>
+  <si>
+    <t>kontrollieren</t>
+  </si>
+  <si>
+    <t>allumer la lumière</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>pisser</t>
+  </si>
+  <si>
+    <t>sauter</t>
+  </si>
+  <si>
+    <t>fermer les rideaux</t>
+  </si>
+  <si>
+    <t>influence</t>
+  </si>
+  <si>
+    <t>empathique</t>
+  </si>
+  <si>
+    <t>das Licht einschalten</t>
+  </si>
+  <si>
+    <t>beenden</t>
+  </si>
+  <si>
+    <t>pissen</t>
+  </si>
+  <si>
+    <t>springen</t>
+  </si>
+  <si>
+    <t>die Vorhänge schliessen</t>
+  </si>
+  <si>
+    <t>le jeu vidéo</t>
+  </si>
+  <si>
+    <t>das Videospiel</t>
+  </si>
+  <si>
+    <t>der Einfluss</t>
+  </si>
+  <si>
+    <t>einfühlsam</t>
+  </si>
+  <si>
+    <t>se réveiller</t>
+  </si>
+  <si>
+    <t>performance</t>
+  </si>
+  <si>
+    <t>finalement</t>
+  </si>
+  <si>
+    <t>la recherche</t>
+  </si>
+  <si>
+    <t>écouter</t>
+  </si>
+  <si>
+    <t>entendre</t>
+  </si>
+  <si>
+    <t>exact</t>
+  </si>
+  <si>
+    <t>investir</t>
+  </si>
+  <si>
+    <t>aufwachen</t>
+  </si>
+  <si>
+    <t>die Leistung</t>
+  </si>
+  <si>
+    <t>die Suche</t>
+  </si>
+  <si>
+    <t>zuhören</t>
+  </si>
+  <si>
+    <t>hören</t>
+  </si>
+  <si>
+    <t>genau</t>
+  </si>
+  <si>
+    <t>investieren</t>
+  </si>
+  <si>
+    <t>structure</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>arrogant</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>adapter</t>
+  </si>
+  <si>
+    <t>pas à pas</t>
+  </si>
+  <si>
+    <t>identifer</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>majorité</t>
+  </si>
+  <si>
+    <t>der Bau</t>
+  </si>
+  <si>
+    <t>das Video</t>
+  </si>
+  <si>
+    <t>le point faible</t>
+  </si>
+  <si>
+    <t>die Schwäche</t>
+  </si>
+  <si>
+    <t>j'ai pensé</t>
+  </si>
+  <si>
+    <t>ich habe gedacht</t>
+  </si>
+  <si>
+    <t>die Basis</t>
+  </si>
+  <si>
+    <t>anpassen</t>
+  </si>
+  <si>
+    <t>Schritt für Schritt</t>
+  </si>
+  <si>
+    <t>erkennen</t>
+  </si>
+  <si>
+    <t>die Quelle</t>
+  </si>
+  <si>
+    <t>die Mehrheit</t>
+  </si>
+  <si>
+    <t>généralement</t>
+  </si>
+  <si>
+    <t>regarder des vidéos</t>
+  </si>
+  <si>
+    <t>paresseux</t>
+  </si>
+  <si>
+    <t>procrastiner</t>
+  </si>
+  <si>
+    <t>terrain</t>
+  </si>
+  <si>
+    <t>ni … ni …</t>
+  </si>
+  <si>
+    <t>C'est parti !</t>
+  </si>
+  <si>
+    <t>Los geht's!</t>
+  </si>
+  <si>
+    <t>se mentir</t>
+  </si>
+  <si>
+    <t>sich selbst belügen</t>
+  </si>
+  <si>
+    <t>Videos anschauen</t>
+  </si>
+  <si>
+    <t>faul</t>
+  </si>
+  <si>
+    <t>aufschieben</t>
+  </si>
+  <si>
+    <t>das Gelände</t>
+  </si>
+  <si>
+    <t>weder … noch …</t>
+  </si>
+  <si>
+    <t>déjà fait</t>
+  </si>
+  <si>
+    <t>prendre soin de soi</t>
+  </si>
+  <si>
+    <t>schon</t>
+  </si>
+  <si>
+    <t>um mich kümmern</t>
+  </si>
+  <si>
+    <t>mettre</t>
+  </si>
+  <si>
+    <t>faire caca</t>
+  </si>
+  <si>
+    <t>doux</t>
+  </si>
+  <si>
+    <t>efficace</t>
+  </si>
+  <si>
+    <t>j'aurais pu</t>
+  </si>
+  <si>
+    <t>c'est tout</t>
+  </si>
+  <si>
+    <t>stellen</t>
+  </si>
+  <si>
+    <t>kacken</t>
+  </si>
+  <si>
+    <t>sympathique</t>
+  </si>
+  <si>
+    <t>freundlich</t>
+  </si>
+  <si>
+    <t>weich</t>
+  </si>
+  <si>
+    <t>effektiv</t>
+  </si>
+  <si>
+    <t>ich hätte … können</t>
+  </si>
+  <si>
+    <t>das ist alles</t>
+  </si>
+  <si>
+    <t>arc-en-ciel</t>
+  </si>
+  <si>
+    <t>puissant</t>
+  </si>
+  <si>
+    <t>outil</t>
+  </si>
+  <si>
+    <t>stressé</t>
+  </si>
+  <si>
+    <t>verbe</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>précis</t>
+  </si>
+  <si>
+    <t>inviter</t>
+  </si>
+  <si>
+    <t>se passer / arriver</t>
+  </si>
+  <si>
+    <t>je m'en fiche</t>
+  </si>
+  <si>
+    <t>der Regenbogen</t>
+  </si>
+  <si>
+    <t>das Werkzeug</t>
+  </si>
+  <si>
+    <t>leistungsfähig</t>
+  </si>
+  <si>
+    <t>gestresst</t>
+  </si>
+  <si>
+    <t>das Substantiv</t>
+  </si>
+  <si>
+    <t>das Verb</t>
+  </si>
+  <si>
+    <t>l'inconnu</t>
+  </si>
+  <si>
+    <t>der Fremde</t>
+  </si>
+  <si>
+    <t>präzis</t>
+  </si>
+  <si>
+    <t>einladen</t>
+  </si>
+  <si>
+    <t>passieren</t>
+  </si>
+  <si>
+    <t>es ist mir egal</t>
+  </si>
+  <si>
+    <t>porter</t>
+  </si>
+  <si>
+    <t>tragen</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>de A à Z</t>
+  </si>
+  <si>
+    <t>ce n'est pas grave</t>
+  </si>
+  <si>
+    <t>séduisant</t>
+  </si>
+  <si>
+    <t>pénis</t>
+  </si>
+  <si>
+    <t>morale</t>
+  </si>
+  <si>
+    <t>rejeter</t>
+  </si>
+  <si>
+    <t>réaliser son rêve</t>
+  </si>
+  <si>
+    <t>le rapport / le ratio</t>
+  </si>
+  <si>
+    <t>das Verhältnis</t>
+  </si>
+  <si>
+    <t>der Ausdruck</t>
+  </si>
+  <si>
+    <t>von A bis Z</t>
+  </si>
+  <si>
+    <t>se tromper</t>
+  </si>
+  <si>
+    <t>sich irren</t>
+  </si>
+  <si>
+    <t>das macht nichts</t>
+  </si>
+  <si>
+    <t>verführerisch</t>
+  </si>
+  <si>
+    <t>der Penis</t>
+  </si>
+  <si>
+    <t>die Moral</t>
+  </si>
+  <si>
+    <t>ablehnen</t>
+  </si>
+  <si>
+    <t>seinen Traum verwirklichen</t>
+  </si>
+  <si>
+    <t>réagir à quelque chose</t>
+  </si>
+  <si>
+    <t>auf etwas reagiren</t>
+  </si>
+  <si>
+    <t>rentrer</t>
+  </si>
+  <si>
+    <t>respecter</t>
+  </si>
+  <si>
+    <t>expressif</t>
+  </si>
+  <si>
+    <t>il est comme ça</t>
+  </si>
+  <si>
+    <t>tirer</t>
+  </si>
+  <si>
+    <t>ziehen</t>
+  </si>
+  <si>
+    <t>es ist klar</t>
+  </si>
+  <si>
+    <t>c'est clair</t>
+  </si>
+  <si>
+    <t>zurückkommen</t>
+  </si>
+  <si>
+    <t>runter</t>
+  </si>
+  <si>
+    <t>respektieren</t>
+  </si>
+  <si>
+    <t>ausdrucksstark</t>
+  </si>
+  <si>
+    <t>so ist er halt</t>
+  </si>
+  <si>
+    <t>die Gelegenheit</t>
+  </si>
+  <si>
+    <t>das Verhalten</t>
+  </si>
+  <si>
+    <t>l'opportunité</t>
+  </si>
+  <si>
+    <t>le comportement</t>
+  </si>
+  <si>
+    <t>il en fait des tonnes</t>
+  </si>
+  <si>
+    <t>ça sent fort</t>
+  </si>
+  <si>
+    <t>continuer</t>
+  </si>
+  <si>
+    <t>fréquent</t>
+  </si>
+  <si>
+    <t>tombé</t>
+  </si>
+  <si>
+    <t>er trägt dick auf</t>
+  </si>
+  <si>
+    <t>der Geruch</t>
+  </si>
+  <si>
+    <t>l'odeur</t>
+  </si>
+  <si>
+    <t>es riecht stark</t>
+  </si>
+  <si>
+    <t>weitermachen</t>
+  </si>
+  <si>
+    <t>häufig</t>
+  </si>
+  <si>
+    <t>am meisten</t>
+  </si>
+  <si>
+    <t>le plus</t>
+  </si>
+  <si>
+    <t>gefallen</t>
+  </si>
+  <si>
+    <t>tourner une vidéo</t>
+  </si>
+  <si>
+    <t>überall</t>
+  </si>
+  <si>
+    <t>puer</t>
+  </si>
+  <si>
+    <t>ligne</t>
+  </si>
+  <si>
+    <t>colonne</t>
+  </si>
+  <si>
+    <t>ein Video drehen</t>
+  </si>
+  <si>
+    <t>partout</t>
+  </si>
+  <si>
+    <t>stinken</t>
+  </si>
+  <si>
+    <t>die Spalte</t>
+  </si>
+  <si>
+    <t>die Zeile</t>
+  </si>
+  <si>
+    <t>masser</t>
+  </si>
+  <si>
+    <t>répondre</t>
+  </si>
+  <si>
+    <t>je me demande</t>
+  </si>
+  <si>
+    <t>ich frage mich</t>
+  </si>
+  <si>
+    <t>massieren</t>
+  </si>
+  <si>
+    <t>antworten</t>
+  </si>
+  <si>
+    <t>pédagogue</t>
+  </si>
+  <si>
+    <t>prononciation</t>
+  </si>
+  <si>
+    <t>prononcer</t>
+  </si>
+  <si>
+    <t>comme d'habitude</t>
+  </si>
+  <si>
+    <t>ausfühlen</t>
+  </si>
+  <si>
+    <t>d'habitude</t>
+  </si>
+  <si>
+    <t>prêté (livre)</t>
+  </si>
+  <si>
+    <t>pädagogisch</t>
+  </si>
+  <si>
+    <t>Kinder zeugen</t>
+  </si>
+  <si>
+    <t>faire des enfants</t>
+  </si>
+  <si>
+    <t>die Aussprache</t>
+  </si>
+  <si>
+    <t>aussprechen</t>
+  </si>
+  <si>
+    <t>wie immer</t>
+  </si>
+  <si>
+    <t>normalerweise</t>
+  </si>
+  <si>
+    <t>das Formular ausfüllen</t>
+  </si>
+  <si>
+    <t>leihen (Buch)</t>
+  </si>
+  <si>
+    <t>retour au source</t>
+  </si>
+  <si>
+    <t>se ressourcer</t>
+  </si>
+  <si>
+    <t>s'habituer</t>
+  </si>
+  <si>
+    <t>changer</t>
+  </si>
+  <si>
+    <t>die Batterien aufladen</t>
+  </si>
+  <si>
+    <t>die Rückkehr zu den Ursprüngen</t>
+  </si>
+  <si>
+    <t>die Reihenfolge</t>
+  </si>
+  <si>
+    <t>l'ordre</t>
+  </si>
+  <si>
+    <t>sich gewöhnen</t>
+  </si>
+  <si>
+    <t>übrigens</t>
+  </si>
+  <si>
+    <t>le seul risque</t>
+  </si>
+  <si>
+    <t>au fait</t>
+  </si>
+  <si>
+    <t>impérativement</t>
+  </si>
+  <si>
+    <t>être parano</t>
+  </si>
+  <si>
+    <t>an Paranoia leiden</t>
+  </si>
+  <si>
+    <t>particulièrement</t>
+  </si>
+  <si>
+    <t>das einzige Risiko</t>
+  </si>
+  <si>
+    <t>avoir le niveau</t>
+  </si>
+  <si>
+    <t>confondre</t>
+  </si>
+  <si>
+    <t>quitter</t>
+  </si>
+  <si>
+    <t>bizarre</t>
+  </si>
+  <si>
+    <t>rentrer dans ma tête</t>
+  </si>
+  <si>
+    <t>das Niveau haben</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>breit</t>
+  </si>
+  <si>
+    <t>verwechseln</t>
+  </si>
+  <si>
+    <t>verlassen</t>
+  </si>
+  <si>
+    <t>seltsam</t>
+  </si>
+  <si>
+    <t>in meinen Kopf bekommen</t>
+  </si>
+  <si>
+    <t>sécher</t>
+  </si>
+  <si>
+    <t>avoir la flemme</t>
+  </si>
+  <si>
+    <t>se masturber</t>
+  </si>
+  <si>
+    <t>je préfère faire que faire</t>
+  </si>
+  <si>
+    <t>trocknen</t>
+  </si>
+  <si>
+    <t>faul sein</t>
+  </si>
+  <si>
+    <t>die Selbstbefriedigung</t>
+  </si>
+  <si>
+    <t>ich mache lieber als machen</t>
+  </si>
+  <si>
+    <t>en train de nettoyer</t>
+  </si>
+  <si>
+    <t>der Angriff</t>
+  </si>
+  <si>
+    <t>l'attaque</t>
+  </si>
+  <si>
+    <t>la conversation</t>
+  </si>
+  <si>
+    <t>das Gespräch</t>
+  </si>
+  <si>
+    <t>gerade putzen</t>
+  </si>
+  <si>
+    <t>je suis jeune</t>
+  </si>
+  <si>
+    <t>la jeunesse</t>
+  </si>
+  <si>
+    <t>l'imagination</t>
+  </si>
+  <si>
+    <t>die Vorstellungskraft</t>
+  </si>
+  <si>
+    <t>la visualisation</t>
+  </si>
+  <si>
+    <t>die Visualisierung</t>
+  </si>
+  <si>
+    <t>ich bin jung</t>
+  </si>
+  <si>
+    <t>die Jugend</t>
+  </si>
+  <si>
+    <t>einen Bug reproduzieren</t>
+  </si>
+  <si>
+    <t>reproduire un bug</t>
+  </si>
+  <si>
+    <t>das Thema</t>
+  </si>
+  <si>
+    <t>le sujet</t>
+  </si>
+  <si>
+    <t>complimenter</t>
+  </si>
+  <si>
+    <t>participer</t>
+  </si>
+  <si>
+    <t>code de la route</t>
+  </si>
+  <si>
+    <t>formation</t>
+  </si>
+  <si>
+    <t>beglückwünschen</t>
+  </si>
+  <si>
+    <t>beteiligen</t>
+  </si>
+  <si>
+    <t>die Strassenverkehrsordnung</t>
+  </si>
+  <si>
+    <t>das Training</t>
+  </si>
+  <si>
+    <t>se forcer à faire quelque chose</t>
+  </si>
+  <si>
+    <t>le vocabulaire</t>
+  </si>
+  <si>
+    <t>point fort</t>
+  </si>
+  <si>
+    <t>passer du temps</t>
+  </si>
+  <si>
+    <t>sich zwingen, etwas zu tun</t>
+  </si>
+  <si>
+    <t>der Wortschatz</t>
+  </si>
+  <si>
+    <t>die Stärke</t>
+  </si>
+  <si>
+    <t>die Zeit verbringen</t>
+  </si>
+  <si>
+    <t>gâcher de la nourriture</t>
+  </si>
+  <si>
+    <t>occuper mes pensées</t>
+  </si>
+  <si>
+    <t>être à l'aise</t>
+  </si>
+  <si>
+    <t>relation amoureuse</t>
+  </si>
+  <si>
+    <t>caissière</t>
+  </si>
+  <si>
+    <t>immeuble</t>
+  </si>
+  <si>
+    <t>Lebensmittel verschwenden</t>
+  </si>
+  <si>
+    <t>le conflit</t>
+  </si>
+  <si>
+    <t>der Konflikt</t>
+  </si>
+  <si>
+    <t>meine Gedanken beschäftigen</t>
+  </si>
+  <si>
+    <t>wohl fühlen</t>
+  </si>
+  <si>
+    <t>die romantische Beziehung</t>
+  </si>
+  <si>
+    <t>das Gebäude</t>
+  </si>
+  <si>
+    <t>die Kassiererin</t>
+  </si>
+  <si>
+    <t>se rendre compte</t>
+  </si>
+  <si>
+    <t>évidemment</t>
+  </si>
+  <si>
+    <t>der Smalltalk</t>
+  </si>
+  <si>
+    <t>le small talk</t>
+  </si>
+  <si>
+    <t>merken</t>
+  </si>
+  <si>
+    <t>natürlich</t>
+  </si>
+  <si>
+    <t>das Gleichgewicht, e</t>
+  </si>
+  <si>
+    <t>l'équilibre</t>
+  </si>
+  <si>
+    <t>tief blicken lassen</t>
+  </si>
+  <si>
+    <t>être révélateur</t>
+  </si>
+  <si>
+    <t>der Ziegelstein, e</t>
+  </si>
+  <si>
+    <t>la brique</t>
+  </si>
+  <si>
+    <t>das liegt daran, dass…</t>
+  </si>
+  <si>
+    <t>c'est dû au fait que…</t>
   </si>
 </sst>
 </file>
@@ -2177,10 +3212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B305"/>
+  <dimension ref="A1:B482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="A306" sqref="A306"/>
+    <sheetView tabSelected="1" topLeftCell="A464" workbookViewId="0">
+      <selection activeCell="A483" sqref="A483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4629,6 +5664,1422 @@
         <v>605</v>
       </c>
     </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A306" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A307" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A308" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A309" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A310" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A311" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A312" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A313" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A314" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A315" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A316" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A317" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A318" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A319" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A320" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A321" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A322" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A323" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A324" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A325" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A326" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A327" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A328" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A329" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A330" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A331" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A332" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A333" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A334" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A335" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A336" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A337" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A338" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A339" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A340" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A341" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A342" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A343" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A344" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A345" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A346" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A347" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A348" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A349" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A350" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A351" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A352" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A353" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A354" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A355" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A356" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A359" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A360" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A362" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A363" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A364" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A365" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A366" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A367" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A368" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A369" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A370" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A371" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A372" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A373" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A374" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A375" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A376" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A377" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A378" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A379" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A380" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A381" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A382" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A383" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A384" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A385" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A386" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A387" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A388" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A389" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A390" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A391" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A392" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A393" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A394" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A395" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A396" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A397" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A398" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A399" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A400" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A401" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A402" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A403" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A404" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A405" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A406" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A407" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A408" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A409" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A410" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A411" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A412" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A413" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A414" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A415" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A416" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A417" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A418" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A419" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A420" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A421" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A422" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A423" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A424" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A425" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A426" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A427" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A428" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A429" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A430" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A431" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A432" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A433" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A434" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B434" s="1" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A435" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A436" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A437" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A438" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A439" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B439" s="1" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A440" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B440" s="1" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A441" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A442" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="B442" s="1" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A443" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B443" s="1" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A444" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A445" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="B445" s="1" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A446" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B446" s="1" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A447" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A448" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A449" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A450" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A451" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A452" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A453" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A454" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A455" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A456" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A457" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A458" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A459" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A460" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A461" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A462" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A463" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A464" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A465" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="B465" s="1" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A466" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A467" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A468" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B468" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A469" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B469" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A470" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A471" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B471" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A472" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="B472" s="1" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A473" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="B473" s="1" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A474" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="B474" s="1" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A475" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A476" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B476" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A477" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A478" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A479" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A480" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="B480" s="1" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A481" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="B481" s="1" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A482" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="B482" s="1" t="s">
+        <v>950</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>